<commit_message>
Incluidos comentários e avaliação semana 1.
</commit_message>
<xml_diff>
--- a/documentacao/G5_Atividades2sem2014.xlsx
+++ b/documentacao/G5_Atividades2sem2014.xlsx
@@ -9,14 +9,15 @@
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
     <sheet name="Semana 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Semana 2" sheetId="4" r:id="rId3"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Atividades</t>
   </si>
@@ -100,6 +101,27 @@
   </si>
   <si>
     <t>Waldinei Pereira da Silva</t>
+  </si>
+  <si>
+    <t>Resultado Final Semana</t>
+  </si>
+  <si>
+    <t>2.4 Requisitos Não Funcionais do Produto</t>
+  </si>
+  <si>
+    <t>2.3 Requisitos Funcionais do Produto</t>
+  </si>
+  <si>
+    <t>2.2 Visão Geral do Produto</t>
+  </si>
+  <si>
+    <t>2.1 Descrições dos Envolvidos e Usuários</t>
+  </si>
+  <si>
+    <t>Descrever e rever a visão do sistema através dos requisitos funcionais e não funcionais.</t>
+  </si>
+  <si>
+    <t>Semana 2</t>
   </si>
 </sst>
 </file>
@@ -303,6 +325,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -333,8 +362,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -344,19 +379,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,7 +696,7 @@
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="5">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
@@ -688,15 +710,15 @@
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="7" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
@@ -707,57 +729,57 @@
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -776,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,76 +819,76 @@
       </c>
     </row>
     <row r="4" spans="2:14" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
       <c r="N11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
       <c r="G12" s="2" t="s">
         <v>4</v>
       </c>
@@ -875,13 +897,13 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="1" t="s">
         <v>5</v>
       </c>
@@ -890,13 +912,13 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="1" t="s">
         <v>5</v>
       </c>
@@ -905,36 +927,40 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="1"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="1"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -958,6 +984,185 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:N17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="N11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1"/>
+      <c r="N13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="1"/>
+      <c r="N14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B4:G9"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G17">
+      <formula1>$N$11:$N$14</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>